<commit_message>
Finished the Excel Dump Utilitiies
</commit_message>
<xml_diff>
--- a/excel_dump.xlsx
+++ b/excel_dump.xlsx
@@ -24,42 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>excel_table</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Sue</t>
-  </si>
-  <si>
-    <t>clock</t>
-  </si>
-  <si>
     <t>row1</t>
   </si>
   <si>
-    <t>xtra</t>
-  </si>
-  <si>
-    <t>onemore</t>
+    <t>s</t>
+  </si>
+  <si>
+    <t>tkb_testing_scraptemp</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -377,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,119 +370,75 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6686</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3.45</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6729</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2.75</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4900</v>
       </c>
       <c r="B5">
         <v>30</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4916</v>
       </c>
       <c r="B6">
         <v>40</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>21</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+        <v>1.88</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>